<commit_message>
finish tech, start dress, add drop down
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wsp/Documents/GitHub/cdfs-performance-rehearsal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BCAF181-5BB1-254A-A2DC-3CFDBA2CF65F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{010870BF-09C5-C745-A416-6840A13F752E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16180" yWindow="2120" windowWidth="23760" windowHeight="20560" activeTab="1" xr2:uid="{2F8600CA-3986-EE4C-91BB-F9BD073B8F74}"/>
+    <workbookView xWindow="21600" yWindow="2120" windowWidth="18340" windowHeight="20560" activeTab="1" xr2:uid="{2F8600CA-3986-EE4C-91BB-F9BD073B8F74}"/>
   </bookViews>
   <sheets>
     <sheet name="classes" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="119">
   <si>
     <t>class_name</t>
   </si>
@@ -355,16 +355,63 @@
   </si>
   <si>
     <t>https://www.cdandfs.com/tech-rehearsals.html</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>Studio</t>
+  </si>
+  <si>
+    <t>Barre Opera House</t>
+  </si>
+  <si>
+    <t>Ballet 2 and Ballet 5 dancers are released at 3:15 pm</t>
+  </si>
+  <si>
+    <t>Pointe 3, Contemporary Ballet, and Ballet 6 dancers are released at 6:15 pm</t>
+  </si>
+  <si>
+    <t>Teen Jazz -- Blackbird</t>
+  </si>
+  <si>
+    <t>Dancers are released to the lobby for pictures after their rehearsal</t>
+  </si>
+  <si>
+    <t>Jazz 2/3</t>
+  </si>
+  <si>
+    <t>Fusion</t>
+  </si>
+  <si>
+    <t>Dress Rehearsal</t>
+  </si>
+  <si>
+    <t>Onstage warm-up for Ballet 4, 5, &amp; 6</t>
+  </si>
+  <si>
+    <t>https://www.cdandfs.com/dress-rehearsals.html</t>
+  </si>
+  <si>
+    <t>Dress Rehearsal: To the Stars: The Ballet Half</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -387,15 +434,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -728,10 +778,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67BBEBB3-3D05-3F4B-827E-9D2E3EA23827}">
-  <dimension ref="A1:E57"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A37" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -786,12 +836,7 @@
       <c r="B6" t="s">
         <v>57</v>
       </c>
-      <c r="D6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0.73958333333333337</v>
-      </c>
+      <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -1424,6 +1469,34 @@
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>113</v>
+      </c>
+      <c r="B58" t="s">
+        <v>67</v>
+      </c>
+      <c r="D58" t="s">
+        <v>68</v>
+      </c>
+      <c r="E58" s="1">
+        <v>0.69791666666666663</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>114</v>
+      </c>
+      <c r="B59" t="s">
+        <v>38</v>
+      </c>
+      <c r="D59" t="s">
+        <v>39</v>
+      </c>
+      <c r="E59" s="1">
+        <v>0.76041666666666663</v>
       </c>
     </row>
   </sheetData>
@@ -1433,24 +1506,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC68AC5E-2942-7D46-915F-1C0B141C9C75}">
-  <dimension ref="A1:H83"/>
+  <dimension ref="A1:I144"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A110" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A134" sqref="A134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.1640625" customWidth="1"/>
     <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" customWidth="1"/>
-    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5" customWidth="1"/>
-    <col min="7" max="7" width="59.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" customWidth="1"/>
+    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5" customWidth="1"/>
+    <col min="8" max="8" width="59.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>88</v>
       </c>
@@ -1458,1873 +1532,3654 @@
         <v>89</v>
       </c>
       <c r="C1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>90</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>91</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>92</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>94</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>93</v>
       </c>
       <c r="B2" s="2">
         <v>45780</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>0.375</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>0.38541666666666669</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>0.36458333333333331</v>
       </c>
-      <c r="H2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>93</v>
       </c>
       <c r="B3" s="2">
         <v>45780</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>0.38541666666666669</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="1">
         <v>0.39583333333333331</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <v>0.36458333333333331</v>
       </c>
-      <c r="H3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>93</v>
       </c>
       <c r="B4" s="2">
         <v>45780</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>0.39583333333333331</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="1">
         <v>0.40625</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
         <v>0.375</v>
       </c>
-      <c r="H4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>93</v>
       </c>
       <c r="B5" s="2">
         <v>45780</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>0.40625</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F5" s="1">
         <v>0.41319444444444442</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="1">
         <v>0.39583333333333331</v>
       </c>
-      <c r="H5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>93</v>
       </c>
       <c r="B6" s="2">
         <v>45780</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>0.41319444444444442</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <v>0.42708333333333331</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G6" s="1">
         <v>0.40625</v>
       </c>
-      <c r="H6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>93</v>
       </c>
       <c r="B7" s="2">
         <v>45780</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D7" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <v>0.42708333333333331</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="1">
         <v>0.44097222222222221</v>
       </c>
-      <c r="H7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>93</v>
       </c>
       <c r="B8" s="2">
         <v>45780</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D8" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <v>0.43055555555555558</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F8" s="1">
         <v>0.44097222222222221</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>95</v>
       </c>
-      <c r="H8" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>93</v>
       </c>
       <c r="B9" s="2">
         <v>45780</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D9" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E9" s="1">
         <v>0.43055555555555558</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9" s="1">
         <v>0.44097222222222221</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>95</v>
       </c>
-      <c r="H9" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>93</v>
       </c>
       <c r="B10" s="2">
         <v>45780</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D10" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="1">
+      <c r="E10" s="1">
         <v>0.43055555555555558</v>
       </c>
-      <c r="E10" s="1">
+      <c r="F10" s="1">
         <v>0.44097222222222221</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>95</v>
       </c>
-      <c r="H10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>93</v>
       </c>
       <c r="B11" s="2">
         <v>45780</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D11" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="1">
+      <c r="E11" s="1">
         <v>0.43055555555555558</v>
       </c>
-      <c r="E11" s="1">
+      <c r="F11" s="1">
         <v>0.44097222222222221</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>95</v>
       </c>
-      <c r="H11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>93</v>
       </c>
       <c r="B12" s="2">
         <v>45780</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D12" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="1">
+      <c r="E12" s="1">
         <v>0.43055555555555558</v>
       </c>
-      <c r="E12" s="1">
+      <c r="F12" s="1">
         <v>0.44097222222222221</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>95</v>
       </c>
-      <c r="H12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>93</v>
       </c>
       <c r="B13" s="2">
         <v>45780</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D13" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="1">
+      <c r="E13" s="1">
         <v>0.43055555555555558</v>
       </c>
-      <c r="E13" s="1">
+      <c r="F13" s="1">
         <v>0.44097222222222221</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>95</v>
       </c>
-      <c r="H13" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>93</v>
       </c>
       <c r="B14" s="2">
         <v>45780</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D14" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="1">
+      <c r="E14" s="1">
         <v>0.4375</v>
       </c>
-      <c r="E14" s="1">
+      <c r="F14" s="1">
         <v>0.4513888888888889</v>
       </c>
-      <c r="H14" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>93</v>
       </c>
       <c r="B15" s="2">
         <v>45780</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D15" t="s">
         <v>80</v>
       </c>
-      <c r="D15" s="1">
+      <c r="E15" s="1">
         <v>0.4513888888888889</v>
       </c>
-      <c r="E15" s="1">
+      <c r="F15" s="1">
         <v>0.45833333333333331</v>
       </c>
-      <c r="H15" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>93</v>
       </c>
       <c r="B16" s="2">
         <v>45780</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D16" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="1">
+      <c r="E16" s="1">
         <v>0.45833333333333331</v>
       </c>
-      <c r="E16" s="1">
+      <c r="F16" s="1">
         <v>0.46527777777777779</v>
       </c>
-      <c r="F16" s="1"/>
-      <c r="H16" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G16" s="1"/>
+      <c r="I16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>93</v>
       </c>
       <c r="B17" s="2">
         <v>45780</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D17" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="1">
+      <c r="E17" s="1">
         <v>0.46527777777777779</v>
       </c>
-      <c r="E17" s="1">
+      <c r="F17" s="1">
         <v>0.47916666666666669</v>
       </c>
-      <c r="F17" s="1">
+      <c r="G17" s="1">
         <v>0.44791666666666669</v>
       </c>
-      <c r="H17" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>93</v>
       </c>
       <c r="B18" s="2">
         <v>45780</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D18" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="1">
+      <c r="E18" s="1">
         <v>0.46875</v>
       </c>
-      <c r="E18" s="1">
+      <c r="F18" s="1">
         <v>0.47916666666666669</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>98</v>
       </c>
-      <c r="H18" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>93</v>
       </c>
       <c r="B19" s="2">
         <v>45780</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D19" t="s">
         <v>80</v>
       </c>
-      <c r="D19" s="1">
+      <c r="E19" s="1">
         <v>0.46875</v>
       </c>
-      <c r="E19" s="1">
+      <c r="F19" s="1">
         <v>0.47916666666666669</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>98</v>
       </c>
-      <c r="H19" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>93</v>
       </c>
       <c r="B20" s="2">
         <v>45780</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D20" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="1">
+      <c r="E20" s="1">
         <v>0.46875</v>
       </c>
-      <c r="E20" s="1">
+      <c r="F20" s="1">
         <v>0.47916666666666669</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>98</v>
       </c>
-      <c r="H20" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I20" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>93</v>
       </c>
       <c r="B21" s="2">
         <v>45780</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D21" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="1">
+      <c r="E21" s="1">
         <v>0.46875</v>
       </c>
-      <c r="E21" s="1">
+      <c r="F21" s="1">
         <v>0.47916666666666669</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>98</v>
       </c>
-      <c r="H21" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I21" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>93</v>
       </c>
       <c r="B22" s="2">
         <v>45780</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D22" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="1">
+      <c r="E22" s="1">
         <v>0.47916666666666669</v>
-      </c>
-      <c r="E22" s="1">
-        <v>0.48958333333333331</v>
       </c>
       <c r="F22" s="1">
         <v>0.48958333333333331</v>
       </c>
-      <c r="H22" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G22" s="1">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="I22" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>93</v>
       </c>
       <c r="B23" s="2">
         <v>45780</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D23" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="1">
+      <c r="E23" s="1">
         <v>0.48958333333333331</v>
       </c>
-      <c r="E23" s="1">
+      <c r="F23" s="1">
         <v>0.5</v>
       </c>
-      <c r="F23" s="1">
+      <c r="G23" s="1">
         <v>0.47916666666666669</v>
       </c>
-      <c r="H23" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I23" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>93</v>
       </c>
       <c r="B24" s="2">
         <v>45780</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D24" t="s">
         <v>78</v>
       </c>
-      <c r="D24" s="1">
+      <c r="E24" s="1">
         <v>0.5</v>
       </c>
-      <c r="E24" s="1">
+      <c r="F24" s="1">
         <v>0.50694444444444442</v>
       </c>
-      <c r="H24" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>93</v>
       </c>
       <c r="B25" s="2">
         <v>45780</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D25" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="1">
+      <c r="E25" s="1">
         <v>0.50694444444444442</v>
       </c>
-      <c r="E25" s="1">
+      <c r="F25" s="1">
         <v>0.51736111111111116</v>
       </c>
-      <c r="H25" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I25" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>93</v>
       </c>
       <c r="B26" s="2">
         <v>45780</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D26" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="1">
+      <c r="E26" s="1">
         <v>0.51736111111111116</v>
       </c>
-      <c r="E26" s="1">
+      <c r="F26" s="1">
         <v>0.52777777777777779</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>97</v>
       </c>
-      <c r="H26" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I26" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>93</v>
       </c>
       <c r="B27" s="2">
         <v>45780</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D27" t="s">
         <v>11</v>
       </c>
-      <c r="D27" s="1">
+      <c r="E27" s="1">
         <v>0.51736111111111116</v>
       </c>
-      <c r="E27" s="1">
+      <c r="F27" s="1">
         <v>0.52777777777777779</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>97</v>
       </c>
-      <c r="H27" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I27" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>93</v>
       </c>
       <c r="B28" s="2">
         <v>45780</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D28" t="s">
         <v>78</v>
       </c>
-      <c r="D28" s="1">
+      <c r="E28" s="1">
         <v>0.51736111111111116</v>
       </c>
-      <c r="E28" s="1">
+      <c r="F28" s="1">
         <v>0.52777777777777779</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>97</v>
       </c>
-      <c r="H28" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I28" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>93</v>
       </c>
       <c r="B29" s="2">
         <v>45780</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D29" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="1">
+      <c r="E29" s="1">
         <v>0.51736111111111116</v>
       </c>
-      <c r="E29" s="1">
+      <c r="F29" s="1">
         <v>0.52777777777777779</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>97</v>
       </c>
-      <c r="H29" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>93</v>
       </c>
       <c r="B30" s="2">
         <v>45780</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D30" t="s">
         <v>5</v>
       </c>
-      <c r="D30" s="1">
+      <c r="E30" s="1">
         <v>0.55208333333333337</v>
       </c>
-      <c r="E30" s="1">
+      <c r="F30" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>100</v>
       </c>
-      <c r="H30" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I30" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>93</v>
       </c>
       <c r="B31" s="2">
         <v>45780</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D31" t="s">
         <v>6</v>
       </c>
-      <c r="D31" s="1">
+      <c r="E31" s="1">
         <v>0.55208333333333337</v>
       </c>
-      <c r="E31" s="1">
+      <c r="F31" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>100</v>
       </c>
-      <c r="H31" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I31" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>93</v>
       </c>
       <c r="B32" s="2">
         <v>45780</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D32" t="s">
         <v>7</v>
       </c>
-      <c r="D32" s="1">
+      <c r="E32" s="1">
         <v>0.55208333333333337</v>
       </c>
-      <c r="E32" s="1">
+      <c r="F32" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>100</v>
       </c>
-      <c r="H32" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I32" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>93</v>
       </c>
       <c r="B33" s="2">
         <v>45780</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D33" t="s">
         <v>8</v>
       </c>
-      <c r="D33" s="1">
+      <c r="E33" s="1">
         <v>0.55208333333333337</v>
       </c>
-      <c r="E33" s="1">
+      <c r="F33" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>100</v>
       </c>
-      <c r="H33" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I33" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>93</v>
       </c>
       <c r="B34" s="2">
         <v>45780</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D34" t="s">
         <v>4</v>
       </c>
-      <c r="D34" s="1">
+      <c r="E34" s="1">
         <v>0.55208333333333337</v>
       </c>
-      <c r="E34" s="1">
+      <c r="F34" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>100</v>
       </c>
-      <c r="H34" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I34" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>93</v>
       </c>
       <c r="B35" s="2">
         <v>45780</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D35" t="s">
         <v>9</v>
       </c>
-      <c r="D35" s="1">
+      <c r="E35" s="1">
         <v>0.55208333333333337</v>
       </c>
-      <c r="E35" s="1">
+      <c r="F35" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="G35" t="s">
+      <c r="H35" t="s">
         <v>100</v>
       </c>
-      <c r="H35" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I35" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>93</v>
       </c>
       <c r="B36" s="2">
         <v>45780</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D36" t="s">
         <v>14</v>
       </c>
-      <c r="D36" s="1">
+      <c r="E36" s="1">
         <v>0.55208333333333337</v>
       </c>
-      <c r="E36" s="1">
+      <c r="F36" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="G36" t="s">
+      <c r="H36" t="s">
         <v>100</v>
       </c>
-      <c r="H36" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I36" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>93</v>
       </c>
       <c r="B37" s="2">
         <v>45780</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D37" t="s">
         <v>80</v>
       </c>
-      <c r="D37" s="1">
+      <c r="E37" s="1">
         <v>0.55208333333333337</v>
       </c>
-      <c r="E37" s="1">
+      <c r="F37" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" t="s">
         <v>100</v>
       </c>
-      <c r="H37" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I37" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>93</v>
       </c>
       <c r="B38" s="2">
         <v>45780</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D38" t="s">
         <v>15</v>
       </c>
-      <c r="D38" s="1">
+      <c r="E38" s="1">
         <v>0.55208333333333337</v>
       </c>
-      <c r="E38" s="1">
+      <c r="F38" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="G38" t="s">
+      <c r="H38" t="s">
         <v>100</v>
       </c>
-      <c r="H38" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I38" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>93</v>
       </c>
       <c r="B39" s="2">
         <v>45780</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D39" t="s">
         <v>16</v>
       </c>
-      <c r="D39" s="1">
+      <c r="E39" s="1">
         <v>0.55208333333333337</v>
       </c>
-      <c r="E39" s="1">
+      <c r="F39" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="G39" t="s">
+      <c r="H39" t="s">
         <v>100</v>
       </c>
-      <c r="H39" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I39" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>93</v>
       </c>
       <c r="B40" s="2">
         <v>45780</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D40" t="s">
         <v>10</v>
       </c>
-      <c r="D40" s="1">
+      <c r="E40" s="1">
         <v>0.55208333333333337</v>
       </c>
-      <c r="E40" s="1">
+      <c r="F40" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="G40" t="s">
+      <c r="H40" t="s">
         <v>100</v>
       </c>
-      <c r="H40" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I40" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>93</v>
       </c>
       <c r="B41" s="2">
         <v>45780</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D41" t="s">
         <v>11</v>
       </c>
-      <c r="D41" s="1">
+      <c r="E41" s="1">
         <v>0.55208333333333337</v>
       </c>
-      <c r="E41" s="1">
+      <c r="F41" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="G41" t="s">
+      <c r="H41" t="s">
         <v>100</v>
       </c>
-      <c r="H41" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I41" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>93</v>
       </c>
       <c r="B42" s="2">
         <v>45780</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D42" t="s">
         <v>78</v>
       </c>
-      <c r="D42" s="1">
+      <c r="E42" s="1">
         <v>0.55208333333333337</v>
       </c>
-      <c r="E42" s="1">
+      <c r="F42" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="G42" t="s">
+      <c r="H42" t="s">
         <v>100</v>
       </c>
-      <c r="H42" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I42" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>93</v>
       </c>
       <c r="B43" s="2">
         <v>45780</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D43" t="s">
         <v>13</v>
       </c>
-      <c r="D43" s="1">
+      <c r="E43" s="1">
         <v>0.55208333333333337</v>
       </c>
-      <c r="E43" s="1">
+      <c r="F43" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="G43" t="s">
+      <c r="H43" t="s">
         <v>100</v>
       </c>
-      <c r="H43" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I43" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>93</v>
       </c>
       <c r="B44" s="2">
         <v>45780</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D44" t="s">
         <v>5</v>
       </c>
-      <c r="D44" s="1">
+      <c r="E44" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="E44" s="1">
+      <c r="F44" s="1">
         <v>0.625</v>
       </c>
-      <c r="G44" t="s">
+      <c r="H44" t="s">
         <v>99</v>
       </c>
-      <c r="H44" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I44" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>93</v>
       </c>
       <c r="B45" s="2">
         <v>45780</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D45" t="s">
         <v>6</v>
       </c>
-      <c r="D45" s="1">
+      <c r="E45" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="E45" s="1">
+      <c r="F45" s="1">
         <v>0.625</v>
       </c>
-      <c r="G45" t="s">
+      <c r="H45" t="s">
         <v>99</v>
       </c>
-      <c r="H45" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I45" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>93</v>
       </c>
       <c r="B46" s="2">
         <v>45780</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D46" t="s">
         <v>7</v>
       </c>
-      <c r="D46" s="1">
+      <c r="E46" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="E46" s="1">
+      <c r="F46" s="1">
         <v>0.625</v>
       </c>
-      <c r="G46" t="s">
+      <c r="H46" t="s">
         <v>99</v>
       </c>
-      <c r="H46" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I46" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>93</v>
       </c>
       <c r="B47" s="2">
         <v>45780</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D47" t="s">
         <v>8</v>
       </c>
-      <c r="D47" s="1">
+      <c r="E47" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="E47" s="1">
+      <c r="F47" s="1">
         <v>0.625</v>
       </c>
-      <c r="G47" t="s">
+      <c r="H47" t="s">
         <v>99</v>
       </c>
-      <c r="H47" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I47" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>93</v>
       </c>
       <c r="B48" s="2">
         <v>45780</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D48" t="s">
         <v>4</v>
       </c>
-      <c r="D48" s="1">
+      <c r="E48" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="E48" s="1">
+      <c r="F48" s="1">
         <v>0.625</v>
       </c>
-      <c r="G48" t="s">
+      <c r="H48" t="s">
         <v>99</v>
       </c>
-      <c r="H48" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I48" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>93</v>
       </c>
       <c r="B49" s="2">
         <v>45780</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D49" t="s">
         <v>9</v>
       </c>
-      <c r="D49" s="1">
+      <c r="E49" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="E49" s="1">
+      <c r="F49" s="1">
         <v>0.625</v>
       </c>
-      <c r="G49" t="s">
+      <c r="H49" t="s">
         <v>99</v>
       </c>
-      <c r="H49" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I49" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>93</v>
       </c>
       <c r="B50" s="2">
         <v>45780</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D50" t="s">
         <v>14</v>
       </c>
-      <c r="D50" s="1">
+      <c r="E50" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="E50" s="1">
+      <c r="F50" s="1">
         <v>0.625</v>
       </c>
-      <c r="G50" t="s">
+      <c r="H50" t="s">
         <v>99</v>
       </c>
-      <c r="H50" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I50" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>93</v>
       </c>
       <c r="B51" s="2">
         <v>45780</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D51" t="s">
         <v>80</v>
       </c>
-      <c r="D51" s="1">
+      <c r="E51" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="E51" s="1">
+      <c r="F51" s="1">
         <v>0.625</v>
       </c>
-      <c r="G51" t="s">
+      <c r="H51" t="s">
         <v>99</v>
       </c>
-      <c r="H51" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I51" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>93</v>
       </c>
       <c r="B52" s="2">
         <v>45780</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D52" t="s">
         <v>15</v>
       </c>
-      <c r="D52" s="1">
+      <c r="E52" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="E52" s="1">
+      <c r="F52" s="1">
         <v>0.625</v>
       </c>
-      <c r="G52" t="s">
+      <c r="H52" t="s">
         <v>99</v>
       </c>
-      <c r="H52" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I52" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>93</v>
       </c>
       <c r="B53" s="2">
         <v>45780</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D53" t="s">
         <v>16</v>
       </c>
-      <c r="D53" s="1">
+      <c r="E53" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="E53" s="1">
+      <c r="F53" s="1">
         <v>0.625</v>
       </c>
-      <c r="G53" t="s">
+      <c r="H53" t="s">
         <v>99</v>
       </c>
-      <c r="H53" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I53" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>93</v>
       </c>
       <c r="B54" s="2">
         <v>45780</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D54" t="s">
         <v>10</v>
       </c>
-      <c r="D54" s="1">
+      <c r="E54" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="E54" s="1">
+      <c r="F54" s="1">
         <v>0.625</v>
       </c>
-      <c r="G54" t="s">
+      <c r="H54" t="s">
         <v>99</v>
       </c>
-      <c r="H54" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I54" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>93</v>
       </c>
       <c r="B55" s="2">
         <v>45780</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D55" t="s">
         <v>11</v>
       </c>
-      <c r="D55" s="1">
+      <c r="E55" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="E55" s="1">
+      <c r="F55" s="1">
         <v>0.625</v>
       </c>
-      <c r="G55" t="s">
+      <c r="H55" t="s">
         <v>99</v>
       </c>
-      <c r="H55" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I55" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>93</v>
       </c>
       <c r="B56" s="2">
         <v>45780</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D56" t="s">
         <v>78</v>
       </c>
-      <c r="D56" s="1">
+      <c r="E56" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="E56" s="1">
+      <c r="F56" s="1">
         <v>0.625</v>
       </c>
-      <c r="G56" t="s">
+      <c r="H56" t="s">
         <v>99</v>
       </c>
-      <c r="H56" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I56" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>93</v>
       </c>
       <c r="B57" s="2">
         <v>45780</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D57" t="s">
         <v>13</v>
       </c>
-      <c r="D57" s="1">
+      <c r="E57" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="E57" s="1">
+      <c r="F57" s="1">
         <v>0.625</v>
       </c>
-      <c r="G57" t="s">
+      <c r="H57" t="s">
         <v>99</v>
       </c>
-      <c r="H57" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I57" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>101</v>
       </c>
       <c r="B58" s="2">
         <v>45788</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D58" t="s">
         <v>5</v>
       </c>
-      <c r="D58" s="1">
+      <c r="E58" s="1">
         <v>0.36458333333333331</v>
       </c>
-      <c r="E58" s="1">
+      <c r="F58" s="1">
         <v>0.39583333333333331</v>
       </c>
-      <c r="H58" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I58" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>101</v>
       </c>
       <c r="B59" s="2">
         <v>45788</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D59" t="s">
         <v>6</v>
       </c>
-      <c r="D59" s="1">
+      <c r="E59" s="1">
         <v>0.38541666666666669</v>
       </c>
-      <c r="E59" s="1">
+      <c r="F59" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="H59" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I59" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>101</v>
       </c>
       <c r="B60" s="2">
         <v>45788</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D60" t="s">
         <v>7</v>
       </c>
-      <c r="D60" s="1">
+      <c r="E60" s="1">
         <v>0.40625</v>
       </c>
-      <c r="E60" s="1">
+      <c r="F60" s="1">
         <v>0.4375</v>
       </c>
-      <c r="H60" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I60" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>101</v>
       </c>
       <c r="B61" s="2">
         <v>45788</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D61" t="s">
         <v>8</v>
       </c>
-      <c r="D61" s="1">
+      <c r="E61" s="1">
         <v>0.42708333333333331</v>
       </c>
-      <c r="E61" s="1">
+      <c r="F61" s="1">
         <v>0.44791666666666669</v>
       </c>
-      <c r="H61" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I61" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>101</v>
       </c>
       <c r="B62" s="2">
         <v>45788</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D62" t="s">
         <v>4</v>
       </c>
-      <c r="D62" s="1">
+      <c r="E62" s="1">
         <v>0.4375</v>
       </c>
-      <c r="E62" s="1">
+      <c r="F62" s="1">
         <v>0.46875</v>
       </c>
-      <c r="H62" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I62" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>101</v>
       </c>
       <c r="B63" s="2">
         <v>45788</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D63" t="s">
         <v>9</v>
       </c>
-      <c r="D63" s="1">
+      <c r="E63" s="1">
         <v>0.45833333333333331</v>
       </c>
-      <c r="E63" s="1">
+      <c r="F63" s="1">
         <v>0.47916666666666669</v>
       </c>
-      <c r="H63" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I63" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>101</v>
       </c>
       <c r="B64" s="2">
         <v>45788</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D64" t="s">
         <v>5</v>
       </c>
-      <c r="D64" s="1">
+      <c r="E64" s="1">
         <v>0.47916666666666669</v>
       </c>
-      <c r="E64" s="1">
+      <c r="F64" s="1">
         <v>0.48958333333333331</v>
       </c>
-      <c r="G64" t="s">
-        <v>102</v>
-      </c>
-      <c r="H64" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I64" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>101</v>
       </c>
       <c r="B65" s="2">
         <v>45788</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D65" t="s">
         <v>6</v>
       </c>
-      <c r="D65" s="1">
+      <c r="E65" s="1">
         <v>0.47916666666666669</v>
       </c>
-      <c r="E65" s="1">
+      <c r="F65" s="1">
         <v>0.48958333333333331</v>
       </c>
-      <c r="G65" t="s">
-        <v>102</v>
-      </c>
-      <c r="H65" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I65" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>101</v>
       </c>
       <c r="B66" s="2">
         <v>45788</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D66" t="s">
         <v>7</v>
       </c>
-      <c r="D66" s="1">
+      <c r="E66" s="1">
         <v>0.47916666666666669</v>
       </c>
-      <c r="E66" s="1">
+      <c r="F66" s="1">
         <v>0.48958333333333331</v>
       </c>
-      <c r="G66" t="s">
-        <v>102</v>
-      </c>
-      <c r="H66" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I66" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>101</v>
       </c>
       <c r="B67" s="2">
         <v>45788</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D67" t="s">
         <v>8</v>
       </c>
-      <c r="D67" s="1">
+      <c r="E67" s="1">
         <v>0.47916666666666669</v>
       </c>
-      <c r="E67" s="1">
+      <c r="F67" s="1">
         <v>0.48958333333333331</v>
       </c>
-      <c r="G67" t="s">
-        <v>102</v>
-      </c>
-      <c r="H67" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I67" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>101</v>
       </c>
       <c r="B68" s="2">
         <v>45788</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D68" t="s">
         <v>4</v>
       </c>
-      <c r="D68" s="1">
+      <c r="E68" s="1">
         <v>0.47916666666666669</v>
       </c>
-      <c r="E68" s="1">
+      <c r="F68" s="1">
         <v>0.48958333333333331</v>
       </c>
-      <c r="G68" t="s">
-        <v>102</v>
-      </c>
-      <c r="H68" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I68" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>101</v>
       </c>
       <c r="B69" s="2">
         <v>45788</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D69" t="s">
         <v>9</v>
       </c>
-      <c r="D69" s="1">
+      <c r="E69" s="1">
         <v>0.47916666666666669</v>
       </c>
-      <c r="E69" s="1">
+      <c r="F69" s="1">
         <v>0.48958333333333331</v>
       </c>
-      <c r="G69" t="s">
-        <v>102</v>
-      </c>
-      <c r="H69" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I69" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>101</v>
       </c>
       <c r="B70" s="2">
         <v>45788</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C70" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D70" t="s">
         <v>5</v>
       </c>
-      <c r="D70" s="1">
+      <c r="E70" s="1">
         <v>0.49305555555555558</v>
       </c>
-      <c r="E70" s="1">
+      <c r="F70" s="1">
         <v>0.53125</v>
       </c>
-      <c r="G70" t="s">
-        <v>102</v>
-      </c>
-      <c r="H70" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I70" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>101</v>
       </c>
       <c r="B71" s="2">
         <v>45788</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D71" t="s">
         <v>6</v>
       </c>
-      <c r="D71" s="1">
+      <c r="E71" s="1">
         <v>0.49305555555555558</v>
       </c>
-      <c r="E71" s="1">
+      <c r="F71" s="1">
         <v>0.53125</v>
       </c>
-      <c r="G71" t="s">
+      <c r="H71" t="s">
         <v>102</v>
       </c>
-      <c r="H71" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I71" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>101</v>
       </c>
       <c r="B72" s="2">
         <v>45788</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D72" t="s">
         <v>7</v>
       </c>
-      <c r="D72" s="1">
+      <c r="E72" s="1">
         <v>0.49305555555555558</v>
       </c>
-      <c r="E72" s="1">
+      <c r="F72" s="1">
         <v>0.53125</v>
       </c>
-      <c r="G72" t="s">
+      <c r="H72" t="s">
         <v>102</v>
       </c>
-      <c r="H72" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I72" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>101</v>
       </c>
       <c r="B73" s="2">
         <v>45788</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C73" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D73" t="s">
         <v>8</v>
       </c>
-      <c r="D73" s="1">
+      <c r="E73" s="1">
         <v>0.49305555555555558</v>
       </c>
-      <c r="E73" s="1">
+      <c r="F73" s="1">
         <v>0.53125</v>
       </c>
-      <c r="G73" t="s">
-        <v>102</v>
-      </c>
-      <c r="H73" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I73" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>101</v>
       </c>
       <c r="B74" s="2">
         <v>45788</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D74" t="s">
         <v>4</v>
       </c>
-      <c r="D74" s="1">
+      <c r="E74" s="1">
         <v>0.49305555555555558</v>
       </c>
-      <c r="E74" s="1">
+      <c r="F74" s="1">
         <v>0.53125</v>
       </c>
-      <c r="G74" t="s">
+      <c r="H74" t="s">
         <v>102</v>
       </c>
-      <c r="H74" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I74" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>101</v>
       </c>
       <c r="B75" s="2">
         <v>45788</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D75" t="s">
         <v>9</v>
       </c>
-      <c r="D75" s="1">
+      <c r="E75" s="1">
         <v>0.49305555555555558</v>
       </c>
-      <c r="E75" s="1">
+      <c r="F75" s="1">
         <v>0.53125</v>
       </c>
-      <c r="G75" t="s">
-        <v>102</v>
-      </c>
-      <c r="H75" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I75" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>101</v>
       </c>
       <c r="B76" s="2">
         <v>45788</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D76" t="s">
         <v>14</v>
       </c>
-      <c r="D76" s="1">
+      <c r="E76" s="1">
         <v>0.49305555555555558</v>
       </c>
-      <c r="E76" s="1">
+      <c r="F76" s="1">
         <v>0.53125</v>
       </c>
-      <c r="G76" t="s">
-        <v>102</v>
-      </c>
-      <c r="H76" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I76" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>101</v>
       </c>
       <c r="B77" s="2">
         <v>45788</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C77" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D77" t="s">
         <v>80</v>
       </c>
-      <c r="D77" s="1">
+      <c r="E77" s="1">
         <v>0.49305555555555558</v>
       </c>
-      <c r="E77" s="1">
+      <c r="F77" s="1">
         <v>0.53125</v>
       </c>
-      <c r="G77" t="s">
-        <v>102</v>
-      </c>
-      <c r="H77" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I77" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>101</v>
       </c>
       <c r="B78" s="2">
         <v>45788</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C78" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D78" t="s">
         <v>15</v>
       </c>
-      <c r="D78" s="1">
+      <c r="E78" s="1">
         <v>0.49305555555555558</v>
       </c>
-      <c r="E78" s="1">
+      <c r="F78" s="1">
         <v>0.53125</v>
       </c>
-      <c r="G78" t="s">
-        <v>102</v>
-      </c>
-      <c r="H78" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I78" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>101</v>
       </c>
       <c r="B79" s="2">
         <v>45788</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C79" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D79" t="s">
         <v>16</v>
       </c>
-      <c r="D79" s="1">
+      <c r="E79" s="1">
         <v>0.49305555555555558</v>
       </c>
-      <c r="E79" s="1">
+      <c r="F79" s="1">
         <v>0.53125</v>
       </c>
-      <c r="G79" t="s">
-        <v>102</v>
-      </c>
-      <c r="H79" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I79" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>101</v>
       </c>
       <c r="B80" s="2">
         <v>45788</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C80" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D80" t="s">
         <v>10</v>
       </c>
-      <c r="D80" s="1">
-        <v>0.49305555555555558</v>
-      </c>
       <c r="E80" s="1">
-        <v>0.53125</v>
-      </c>
-      <c r="G80" t="s">
-        <v>102</v>
-      </c>
-      <c r="H80" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F80" s="1">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="I80" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>101</v>
       </c>
       <c r="B81" s="2">
         <v>45788</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C81" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D81" t="s">
         <v>11</v>
       </c>
-      <c r="D81" s="1">
-        <v>0.49305555555555558</v>
-      </c>
       <c r="E81" s="1">
-        <v>0.53125</v>
-      </c>
-      <c r="G81" t="s">
-        <v>102</v>
-      </c>
-      <c r="H81" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0.5625</v>
+      </c>
+      <c r="F81" s="1">
+        <v>0.59375</v>
+      </c>
+      <c r="I81" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>101</v>
       </c>
       <c r="B82" s="2">
         <v>45788</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C82" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D82" t="s">
         <v>78</v>
       </c>
-      <c r="D82" s="1">
-        <v>0.49305555555555558</v>
-      </c>
       <c r="E82" s="1">
-        <v>0.53125</v>
-      </c>
-      <c r="G82" t="s">
-        <v>102</v>
-      </c>
-      <c r="H82" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F82" s="1">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="I82" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>101</v>
       </c>
       <c r="B83" s="2">
         <v>45788</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C83" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D83" t="s">
         <v>13</v>
       </c>
-      <c r="D83" s="1">
-        <v>0.49305555555555558</v>
-      </c>
       <c r="E83" s="1">
-        <v>0.53125</v>
-      </c>
-      <c r="G83" t="s">
-        <v>102</v>
-      </c>
-      <c r="H83" t="s">
-        <v>105</v>
+        <v>0.59375</v>
+      </c>
+      <c r="F83" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="I83" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>101</v>
+      </c>
+      <c r="B84" s="2">
+        <v>45788</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D84" t="s">
+        <v>10</v>
+      </c>
+      <c r="E84" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="F84" s="1">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="H84" t="s">
+        <v>109</v>
+      </c>
+      <c r="I84" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>101</v>
+      </c>
+      <c r="B85" s="2">
+        <v>45788</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D85" t="s">
+        <v>11</v>
+      </c>
+      <c r="E85" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="F85" s="1">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="I85" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>101</v>
+      </c>
+      <c r="B86" s="2">
+        <v>45788</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D86" t="s">
+        <v>78</v>
+      </c>
+      <c r="E86" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="F86" s="1">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="I86" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>101</v>
+      </c>
+      <c r="B87" s="2">
+        <v>45788</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D87" t="s">
+        <v>13</v>
+      </c>
+      <c r="E87" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="F87" s="1">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="H87" t="s">
+        <v>109</v>
+      </c>
+      <c r="I87" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>101</v>
+      </c>
+      <c r="B88" s="2">
+        <v>45788</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D88" t="s">
+        <v>14</v>
+      </c>
+      <c r="E88" s="1">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F88" s="1">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="H88" t="s">
+        <v>110</v>
+      </c>
+      <c r="I88" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>101</v>
+      </c>
+      <c r="B89" s="2">
+        <v>45788</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D89" t="s">
+        <v>80</v>
+      </c>
+      <c r="E89" s="1">
+        <v>0.6875</v>
+      </c>
+      <c r="F89" s="1">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="H89" t="s">
+        <v>110</v>
+      </c>
+      <c r="I89" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>101</v>
+      </c>
+      <c r="B90" s="2">
+        <v>45788</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D90" t="s">
+        <v>15</v>
+      </c>
+      <c r="E90" s="1">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="F90" s="1">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="H90" t="s">
+        <v>110</v>
+      </c>
+      <c r="I90" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>101</v>
+      </c>
+      <c r="B91" s="2">
+        <v>45788</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D91" t="s">
+        <v>16</v>
+      </c>
+      <c r="E91" s="1">
+        <v>0.71875</v>
+      </c>
+      <c r="F91" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="H91" t="s">
+        <v>110</v>
+      </c>
+      <c r="I91" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>101</v>
+      </c>
+      <c r="B92" s="2">
+        <v>45788</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D92" t="s">
+        <v>14</v>
+      </c>
+      <c r="E92" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="F92" s="1">
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="H92" t="s">
+        <v>110</v>
+      </c>
+      <c r="I92" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>101</v>
+      </c>
+      <c r="B93" s="2">
+        <v>45788</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D93" t="s">
+        <v>80</v>
+      </c>
+      <c r="E93" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="F93" s="1">
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="H93" t="s">
+        <v>110</v>
+      </c>
+      <c r="I93" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>101</v>
+      </c>
+      <c r="B94" s="2">
+        <v>45788</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D94" t="s">
+        <v>15</v>
+      </c>
+      <c r="E94" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="F94" s="1">
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="H94" t="s">
+        <v>110</v>
+      </c>
+      <c r="I94" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>101</v>
+      </c>
+      <c r="B95" s="2">
+        <v>45788</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D95" t="s">
+        <v>16</v>
+      </c>
+      <c r="E95" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="F95" s="1">
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="H95" t="s">
+        <v>110</v>
+      </c>
+      <c r="I95" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>101</v>
+      </c>
+      <c r="B96" s="2">
+        <v>45788</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D96" t="s">
+        <v>111</v>
+      </c>
+      <c r="E96" s="1">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="F96" s="1">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="I96" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>101</v>
+      </c>
+      <c r="B97" s="2">
+        <v>45788</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D97" t="s">
+        <v>18</v>
+      </c>
+      <c r="E97" s="1">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="F97" s="1">
+        <v>0.8125</v>
+      </c>
+      <c r="I97" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>101</v>
+      </c>
+      <c r="B98" s="2">
+        <v>45788</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D98" t="s">
+        <v>19</v>
+      </c>
+      <c r="E98" s="1">
+        <v>0.8125</v>
+      </c>
+      <c r="F98" s="1">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="I98" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>101</v>
+      </c>
+      <c r="B99" s="2">
+        <v>45788</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D99" t="s">
+        <v>20</v>
+      </c>
+      <c r="E99" s="1">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="F99" s="1">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="I99" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>101</v>
+      </c>
+      <c r="B100" s="2">
+        <v>45788</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D100" t="s">
+        <v>21</v>
+      </c>
+      <c r="E100" s="1">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="F100" s="1">
+        <v>0.875</v>
+      </c>
+      <c r="I100" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>101</v>
+      </c>
+      <c r="B101" s="2">
+        <v>45788</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D101" t="s">
+        <v>22</v>
+      </c>
+      <c r="E101" s="1">
+        <v>0.875</v>
+      </c>
+      <c r="F101" s="1">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="I101" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>101</v>
+      </c>
+      <c r="B102" s="2">
+        <v>45789</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D102" t="s">
+        <v>43</v>
+      </c>
+      <c r="E102" s="1">
+        <v>0.65625</v>
+      </c>
+      <c r="F102" s="1">
+        <v>0.6875</v>
+      </c>
+      <c r="H102" t="s">
+        <v>112</v>
+      </c>
+      <c r="I102" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>101</v>
+      </c>
+      <c r="B103" s="2">
+        <v>45789</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D103" t="s">
+        <v>45</v>
+      </c>
+      <c r="E103" s="1">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="F103" s="1">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="H103" t="s">
+        <v>112</v>
+      </c>
+      <c r="I103" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>101</v>
+      </c>
+      <c r="B104" s="2">
+        <v>45789</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D104" t="s">
+        <v>46</v>
+      </c>
+      <c r="E104" s="1">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="F104" s="1">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="H104" t="s">
+        <v>112</v>
+      </c>
+      <c r="I104" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>101</v>
+      </c>
+      <c r="B105" s="2">
+        <v>45789</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D105" t="s">
+        <v>47</v>
+      </c>
+      <c r="E105" s="1">
+        <v>0.71875</v>
+      </c>
+      <c r="F105" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="H105" t="s">
+        <v>112</v>
+      </c>
+      <c r="I105" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>101</v>
+      </c>
+      <c r="B106" s="2">
+        <v>45789</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D106" t="s">
+        <v>49</v>
+      </c>
+      <c r="E106" s="1">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="F106" s="1">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="H106" t="s">
+        <v>112</v>
+      </c>
+      <c r="I106" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>101</v>
+      </c>
+      <c r="B107" s="2">
+        <v>45789</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D107" t="s">
+        <v>50</v>
+      </c>
+      <c r="E107" s="1">
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="F107" s="1">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="H107" t="s">
+        <v>112</v>
+      </c>
+      <c r="I107" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>101</v>
+      </c>
+      <c r="B108" s="2">
+        <v>45789</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D108" t="s">
+        <v>51</v>
+      </c>
+      <c r="E108" s="1">
+        <v>0.80555555555555558</v>
+      </c>
+      <c r="F108" s="1">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="H108" t="s">
+        <v>112</v>
+      </c>
+      <c r="I108" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>101</v>
+      </c>
+      <c r="B109" s="2">
+        <v>45789</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D109" t="s">
+        <v>52</v>
+      </c>
+      <c r="E109" s="1">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="F109" s="1">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="H109" t="s">
+        <v>112</v>
+      </c>
+      <c r="I109" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>101</v>
+      </c>
+      <c r="B110" s="2">
+        <v>45789</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D110" t="s">
+        <v>53</v>
+      </c>
+      <c r="E110" s="1">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="F110" s="1">
+        <v>0.875</v>
+      </c>
+      <c r="H110" t="s">
+        <v>112</v>
+      </c>
+      <c r="I110" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>101</v>
+      </c>
+      <c r="B111" s="2">
+        <v>45789</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D111" t="s">
+        <v>54</v>
+      </c>
+      <c r="E111" s="1">
+        <v>0.875</v>
+      </c>
+      <c r="F111" s="1">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="H111" t="s">
+        <v>112</v>
+      </c>
+      <c r="I111" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>101</v>
+      </c>
+      <c r="B112" s="2">
+        <v>45789</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D112" t="s">
+        <v>55</v>
+      </c>
+      <c r="E112" s="1">
+        <v>0.88541666666666663</v>
+      </c>
+      <c r="F112" s="1">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="H112" t="s">
+        <v>112</v>
+      </c>
+      <c r="I112" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>101</v>
+      </c>
+      <c r="B113" s="2">
+        <v>45790</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D113" t="s">
+        <v>60</v>
+      </c>
+      <c r="E113" s="1">
+        <v>0.65625</v>
+      </c>
+      <c r="F113" s="1">
+        <v>0.6875</v>
+      </c>
+      <c r="H113" t="s">
+        <v>112</v>
+      </c>
+      <c r="I113" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>101</v>
+      </c>
+      <c r="B114" s="2">
+        <v>45790</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D114" t="s">
+        <v>62</v>
+      </c>
+      <c r="E114" s="1">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="F114" s="1">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="H114" t="s">
+        <v>112</v>
+      </c>
+      <c r="I114" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>101</v>
+      </c>
+      <c r="B115" s="2">
+        <v>45790</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D115" t="s">
+        <v>64</v>
+      </c>
+      <c r="E115" s="1">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="F115" s="1">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="H115" t="s">
+        <v>112</v>
+      </c>
+      <c r="I115" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>101</v>
+      </c>
+      <c r="B116" s="2">
+        <v>45790</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D116" t="s">
+        <v>65</v>
+      </c>
+      <c r="E116" s="1">
+        <v>0.71875</v>
+      </c>
+      <c r="F116" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="H116" t="s">
+        <v>112</v>
+      </c>
+      <c r="I116" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>101</v>
+      </c>
+      <c r="B117" s="2">
+        <v>45790</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D117" t="s">
+        <v>66</v>
+      </c>
+      <c r="E117" s="1">
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="F117" s="1">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="H117" t="s">
+        <v>112</v>
+      </c>
+      <c r="I117" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>101</v>
+      </c>
+      <c r="B118" s="2">
+        <v>45790</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D118" t="s">
+        <v>69</v>
+      </c>
+      <c r="E118" s="1">
+        <v>0.78125</v>
+      </c>
+      <c r="F118" s="1">
+        <v>0.8125</v>
+      </c>
+      <c r="H118" t="s">
+        <v>112</v>
+      </c>
+      <c r="I118" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>101</v>
+      </c>
+      <c r="B119" s="2">
+        <v>45790</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D119" t="s">
+        <v>70</v>
+      </c>
+      <c r="E119" s="1">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="F119" s="1">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="H119" t="s">
+        <v>112</v>
+      </c>
+      <c r="I119" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>101</v>
+      </c>
+      <c r="B120" s="2">
+        <v>45790</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D120" t="s">
+        <v>113</v>
+      </c>
+      <c r="E120" s="1">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="F120" s="1">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="H120" t="s">
+        <v>112</v>
+      </c>
+      <c r="I120" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>101</v>
+      </c>
+      <c r="B121" s="2">
+        <v>45790</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D121" t="s">
+        <v>71</v>
+      </c>
+      <c r="E121" s="1">
+        <v>0.84375</v>
+      </c>
+      <c r="F121" s="1">
+        <v>0.875</v>
+      </c>
+      <c r="H121" t="s">
+        <v>112</v>
+      </c>
+      <c r="I121" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>101</v>
+      </c>
+      <c r="B122" s="2">
+        <v>45790</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D122" t="s">
+        <v>72</v>
+      </c>
+      <c r="E122" s="1">
+        <v>0.86458333333333337</v>
+      </c>
+      <c r="F122" s="1">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="H122" t="s">
+        <v>112</v>
+      </c>
+      <c r="I122" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>101</v>
+      </c>
+      <c r="B123" s="2">
+        <v>45790</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D123" t="s">
+        <v>74</v>
+      </c>
+      <c r="E123" s="1">
+        <v>0.88541666666666663</v>
+      </c>
+      <c r="F123" s="1">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="H123" t="s">
+        <v>112</v>
+      </c>
+      <c r="I123" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>101</v>
+      </c>
+      <c r="B124" s="2">
+        <v>45791</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D124" t="s">
+        <v>23</v>
+      </c>
+      <c r="E124" s="1">
+        <v>0.65625</v>
+      </c>
+      <c r="F124" s="1">
+        <v>0.6875</v>
+      </c>
+      <c r="H124" t="s">
+        <v>112</v>
+      </c>
+      <c r="I124" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>101</v>
+      </c>
+      <c r="B125" s="2">
+        <v>45791</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D125" t="s">
+        <v>26</v>
+      </c>
+      <c r="E125" s="1">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="F125" s="1">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="H125" t="s">
+        <v>112</v>
+      </c>
+      <c r="I125" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>101</v>
+      </c>
+      <c r="B126" s="2">
+        <v>45791</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D126" t="s">
+        <v>27</v>
+      </c>
+      <c r="E126" s="1">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="F126" s="1">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="H126" t="s">
+        <v>112</v>
+      </c>
+      <c r="I126" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>101</v>
+      </c>
+      <c r="B127" s="2">
+        <v>45791</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D127" t="s">
+        <v>29</v>
+      </c>
+      <c r="E127" s="1">
+        <v>0.71875</v>
+      </c>
+      <c r="F127" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="H127" t="s">
+        <v>112</v>
+      </c>
+      <c r="I127" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>101</v>
+      </c>
+      <c r="B128" s="2">
+        <v>45791</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D128" t="s">
+        <v>32</v>
+      </c>
+      <c r="E128" s="1">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="F128" s="1">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="H128" t="s">
+        <v>112</v>
+      </c>
+      <c r="I128" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>101</v>
+      </c>
+      <c r="B129" s="2">
+        <v>45791</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D129" t="s">
+        <v>34</v>
+      </c>
+      <c r="E129" s="1">
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="F129" s="1">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="H129" t="s">
+        <v>112</v>
+      </c>
+      <c r="I129" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>101</v>
+      </c>
+      <c r="B130" s="2">
+        <v>45791</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D130" t="s">
+        <v>37</v>
+      </c>
+      <c r="E130" s="1">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="F130" s="1">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="H130" t="s">
+        <v>112</v>
+      </c>
+      <c r="I130" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>101</v>
+      </c>
+      <c r="B131" s="2">
+        <v>45791</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D131" t="s">
+        <v>40</v>
+      </c>
+      <c r="E131" s="1">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="F131" s="1">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="H131" t="s">
+        <v>112</v>
+      </c>
+      <c r="I131" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>101</v>
+      </c>
+      <c r="B132" s="2">
+        <v>45791</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D132" t="s">
+        <v>114</v>
+      </c>
+      <c r="E132" s="1">
+        <v>0.84375</v>
+      </c>
+      <c r="F132" s="1">
+        <v>0.875</v>
+      </c>
+      <c r="H132" t="s">
+        <v>112</v>
+      </c>
+      <c r="I132" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>101</v>
+      </c>
+      <c r="B133" s="2">
+        <v>45791</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D133" t="s">
+        <v>59</v>
+      </c>
+      <c r="E133" s="1">
+        <v>0.86458333333333337</v>
+      </c>
+      <c r="F133" s="1">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="H133" t="s">
+        <v>112</v>
+      </c>
+      <c r="I133" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>101</v>
+      </c>
+      <c r="B134" s="2">
+        <v>45791</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D134" t="s">
+        <v>42</v>
+      </c>
+      <c r="E134" s="1">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="F134" s="1">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="H134" t="s">
+        <v>112</v>
+      </c>
+      <c r="I134" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>115</v>
+      </c>
+      <c r="B135" s="2">
+        <v>45792</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D135" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E135" s="1">
+        <v>0.65625</v>
+      </c>
+      <c r="F135" s="1">
+        <v>0.6875</v>
+      </c>
+      <c r="G135" s="1">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="H135" t="s">
+        <v>116</v>
+      </c>
+      <c r="I135" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>115</v>
+      </c>
+      <c r="B136" s="2">
+        <v>45792</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D136" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E136" s="1">
+        <v>0.65625</v>
+      </c>
+      <c r="F136" s="1">
+        <v>0.6875</v>
+      </c>
+      <c r="G136" s="1">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="H136" t="s">
+        <v>116</v>
+      </c>
+      <c r="I136" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>115</v>
+      </c>
+      <c r="B137" s="2">
+        <v>45792</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D137" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E137" s="1">
+        <v>0.65625</v>
+      </c>
+      <c r="F137" s="1">
+        <v>0.6875</v>
+      </c>
+      <c r="G137" s="1">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="H137" t="s">
+        <v>116</v>
+      </c>
+      <c r="I137" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>115</v>
+      </c>
+      <c r="B138" s="2">
+        <v>45792</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D138" t="s">
+        <v>4</v>
+      </c>
+      <c r="E138" s="1">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="F138" s="1">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="G138" s="1">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="H138" t="s">
+        <v>118</v>
+      </c>
+      <c r="I138" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>115</v>
+      </c>
+      <c r="B139" s="2">
+        <v>45792</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D139" t="s">
+        <v>10</v>
+      </c>
+      <c r="E139" s="1">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="F139" s="1">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="G139" s="1">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="H139" t="s">
+        <v>118</v>
+      </c>
+      <c r="I139" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>115</v>
+      </c>
+      <c r="B140" s="2">
+        <v>45792</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D140" t="s">
+        <v>6</v>
+      </c>
+      <c r="E140" s="1">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="F140" s="1">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="G140" s="1">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="H140" t="s">
+        <v>118</v>
+      </c>
+      <c r="I140" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>115</v>
+      </c>
+      <c r="B141" s="2">
+        <v>45792</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D141" t="s">
+        <v>16</v>
+      </c>
+      <c r="E141" s="1">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="F141" s="1">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="G141" s="1">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="H141" t="s">
+        <v>118</v>
+      </c>
+      <c r="I141" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>115</v>
+      </c>
+      <c r="B142" s="2">
+        <v>45792</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D142" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E142" s="1">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="F142" s="1">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="H142" t="s">
+        <v>118</v>
+      </c>
+      <c r="I142" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>115</v>
+      </c>
+      <c r="B143" s="2">
+        <v>45792</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D143" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E143" s="1">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="F143" s="1">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="H143" t="s">
+        <v>118</v>
+      </c>
+      <c r="I143" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>115</v>
+      </c>
+      <c r="B144" s="2">
+        <v>45792</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D144" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E144" s="1">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="F144" s="1">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="H144" t="s">
+        <v>118</v>
+      </c>
+      <c r="I144" s="3" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -3336,7 +5191,7 @@
           <x14:formula1>
             <xm:f>classes!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C83</xm:sqref>
+          <xm:sqref>D2:D134 D138:D141 D145:D370</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
add explicit sort of rehearsals data
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wsp/Documents/GitHub/cdfs-performance-rehearsal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF8DD28-8FC1-2F4D-B53F-AC40A4035F08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{669ED2BA-F786-174E-B728-89D05E9AC524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7360" yWindow="2120" windowWidth="32580" windowHeight="24460" xr2:uid="{2F8600CA-3986-EE4C-91BB-F9BD073B8F74}"/>
+    <workbookView xWindow="7420" yWindow="2360" windowWidth="32580" windowHeight="21100" activeTab="1" xr2:uid="{2F8600CA-3986-EE4C-91BB-F9BD073B8F74}"/>
   </bookViews>
   <sheets>
     <sheet name="classes" sheetId="1" r:id="rId1"/>
@@ -785,7 +785,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67BBEBB3-3D05-3F4B-827E-9D2E3EA23827}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
@@ -1420,8 +1420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC68AC5E-2942-7D46-915F-1C0B141C9C75}">
   <dimension ref="A1:J144"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
@@ -1430,11 +1430,12 @@
     <col min="1" max="1" width="18.1640625" customWidth="1"/>
     <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.6640625" customWidth="1"/>
-    <col min="4" max="5" width="21.6640625" customWidth="1"/>
+    <col min="4" max="4" width="31.33203125" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" customWidth="1"/>
     <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.5" customWidth="1"/>
-    <col min="9" max="9" width="59.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="66" customWidth="1"/>
     <col min="10" max="10" width="48.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>